<commit_message>
reports sub menu changes
reports sub menu changes
</commit_message>
<xml_diff>
--- a/Issue Tracker.xlsx
+++ b/Issue Tracker.xlsx
@@ -172,7 +172,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +183,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -236,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -251,6 +266,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,10 +740,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:Q10"/>
+  <dimension ref="A2:Q20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -741,7 +758,7 @@
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
@@ -964,7 +981,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" ht="28.5">
       <c r="A10">
         <v>6</v>
       </c>
@@ -990,15 +1007,51 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="8">
         <f>(M5+P5)/O5</f>
         <v>176.66666666666666</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="9">
         <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="M13" s="6">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="M14" s="6">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="M15" s="6">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="M16" s="6">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="13:13">
+      <c r="M17" s="6">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="13:13">
+      <c r="M18" s="6">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="13:13">
+      <c r="M20" s="6">
+        <f>SUM(M13:M18)</f>
+        <v>1060</v>
       </c>
     </row>
   </sheetData>

</xml_diff>